<commit_message>
Implement controller and fix the signal table
</commit_message>
<xml_diff>
--- a/cpu/doc/signal_table.xlsx
+++ b/cpu/doc/signal_table.xlsx
@@ -1,26 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wonicon\Desktop\Lab4_131220159_王诲喆_0.3_信号表\cpu\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="Calc"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="229" firstSheet="1" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="229" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="origin" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="transpose" sheetId="2" r:id="rId2"/>
+    <sheet name="origin" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="transpose" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="126">
   <si>
     <t>add</t>
   </si>
@@ -351,225 +347,92 @@
     <t>XB (not use, rt == rd)</t>
   </si>
   <si>
+    <t>instr</t>
+  </si>
+  <si>
+    <t>    Rt_addr_sel</t>
+  </si>
+  <si>
+    <t>0000B (write)</t>
+  </si>
+  <si>
+    <t>1111B (not write)</t>
+  </si>
+  <si>
+    <t>110B (&lt;)</t>
+  </si>
+  <si>
+    <t>011B (&gt;=)</t>
+  </si>
+  <si>
+    <t>001B (=)</t>
+  </si>
+  <si>
+    <t>XB (rd == rt)</t>
+  </si>
+  <si>
+    <t>XB（rd == rt)</t>
+  </si>
+  <si>
+    <t>seh</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
     <t>XXB (not alu)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>XB (not care)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>XXXXB (not calc)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>XB (no writing)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>XB (not calc)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>XXB (not care)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>XXXB (not use)</t>
   </si>
   <si>
     <t>1B (abs jmp)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>XB (not use)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">    Rt_addr_sel</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>instr</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000B (write)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>111</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>B (not write)</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000B (write)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>111</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>B (not write)</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000B (write)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000B (write)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000B (write)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1111B (not write)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1111B (not write)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>0</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>000</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>B (write)</t>
-    </r>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1111B (not write)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1111B (not write)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000B (write)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1111B (not write)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1111B (not write)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>j</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>01B (logical right)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>001B (=)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>011B (&gt;=)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>110B (&lt;)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>000B (no branch)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>XXXB (not use)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>seh</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>XB (rd == rt)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>XB（rd == rt)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <name val="宋体"/>
+      <family val="0"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="10"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
+      <family val="0"/>
       <charset val="134"/>
     </font>
     <font>
@@ -580,7 +443,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color indexed="10"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -595,870 +458,263 @@
     </fill>
   </fills>
   <borders count="8">
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
-        <color indexed="63"/>
+        <color rgb="FF333333"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="63"/>
+        <color rgb="FF333333"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="63"/>
+        <color rgb="FF333333"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin">
-        <color indexed="63"/>
+        <color rgb="FF333333"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
-        <color indexed="63"/>
+        <color rgb="FF333333"/>
       </left>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left style="thin">
-        <color indexed="63"/>
+        <color rgb="FF333333"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="63"/>
+        <color rgb="FF333333"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="63"/>
+        <color rgb="FF333333"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin">
-        <color indexed="63"/>
+        <color rgb="FF333333"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="63"/>
+        <color rgb="FF333333"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
+  <cellXfs count="28">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+  <cellStyles count="6">
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="宋体"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="表1" displayName="表1" ref="A1:M38" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
-  <autoFilter ref="A1:M38"/>
-  <tableColumns count="13">
-    <tableColumn id="1" name="instr" dataDxfId="12"/>
-    <tableColumn id="2" name="Rd_byte_w_en[3:0]_x000a_(Overflow=0)" dataDxfId="11"/>
-    <tableColumn id="3" name="Rd_byte_w_en[3:0]_x000a_(Overflow=1)" dataDxfId="10"/>
-    <tableColumn id="4" name="B_in_sel[1:0]" dataDxfId="9"/>
-    <tableColumn id="5" name="Extend_sel" dataDxfId="8"/>
-    <tableColumn id="6" name="ALU_op[3:0]" dataDxfId="7"/>
-    <tableColumn id="7" name="Rd_addr_sel" dataDxfId="6"/>
-    <tableColumn id="8" name="Shift_amount_sel" dataDxfId="5"/>
-    <tableColumn id="9" name="ALU_Shift_sel" dataDxfId="4"/>
-    <tableColumn id="10" name="condition[2:0]" dataDxfId="3"/>
-    <tableColumn id="11" name="Shift_op[1:0]" dataDxfId="2"/>
-    <tableColumn id="12" name="Jump" dataDxfId="1"/>
-    <tableColumn id="13" name="    Rt_addr_sel" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults>
-    <a:spDef>
-      <a:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1" cy="1"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst/>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
-        </a:solidFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </a:spPr>
-      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
-      <a:lstStyle/>
-    </a:spDef>
-    <a:lnDef>
-      <a:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="1" cy="1"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst/>
-        </a:custGeom>
-        <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
-        </a:solidFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
-        </a:ln>
-        <a:effectLst/>
-        <a:extLst>
-          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:effectLst>
-                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="808080"/>
-                </a:outerShdw>
-              </a:effectLst>
-            </a14:hiddenEffects>
-          </a:ext>
-        </a:extLst>
-      </a:spPr>
-      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
-      <a:lstStyle/>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AN13"/>
   <sheetViews>
-    <sheetView zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="AM19" sqref="AM19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AM19" activeCellId="2" sqref="E12:E22 E23:E25 AM19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="11" width="19" customWidth="1"/>
-    <col min="12" max="13" width="20" style="1" customWidth="1"/>
-    <col min="14" max="15" width="19" customWidth="1"/>
-    <col min="16" max="16" width="22" customWidth="1"/>
-    <col min="17" max="18" width="19" customWidth="1"/>
-    <col min="19" max="19" width="25" customWidth="1"/>
-    <col min="20" max="26" width="20" customWidth="1"/>
-    <col min="27" max="27" width="21" customWidth="1"/>
-    <col min="28" max="28" width="19" customWidth="1"/>
-    <col min="29" max="30" width="24" customWidth="1"/>
-    <col min="31" max="32" width="19" customWidth="1"/>
-    <col min="33" max="40" width="30" customWidth="1"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.9952830188679"/>
+    <col collapsed="false" hidden="false" max="11" min="2" style="0" width="19.0047169811321"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="1" width="20"/>
+    <col collapsed="false" hidden="false" max="15" min="14" style="0" width="19.0047169811321"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="22"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="0" width="19.0047169811321"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="25"/>
+    <col collapsed="false" hidden="false" max="26" min="20" style="0" width="20"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="0" width="21"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="19.0047169811321"/>
+    <col collapsed="false" hidden="false" max="30" min="29" style="0" width="24.0047169811321"/>
+    <col collapsed="false" hidden="false" max="32" min="31" style="0" width="19.0047169811321"/>
+    <col collapsed="false" hidden="false" max="40" min="33" style="0" width="30.0047169811321"/>
+    <col collapsed="false" hidden="false" max="1025" min="41" style="0" width="8.67924528301887"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2"/>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1578,7 +834,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:40" ht="28.5" x14ac:dyDescent="0.15">
+    <row r="2" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>39</v>
       </c>
@@ -1700,7 +956,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:40" ht="28.5" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="12" t="s">
         <v>43</v>
       </c>
@@ -1822,7 +1078,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="14" t="s">
         <v>44</v>
       </c>
@@ -1944,7 +1200,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="s">
         <v>50</v>
       </c>
@@ -2066,7 +1322,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="s">
         <v>53</v>
       </c>
@@ -2188,7 +1444,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="s">
         <v>70</v>
       </c>
@@ -2310,7 +1566,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="14" t="s">
         <v>76</v>
       </c>
@@ -2432,7 +1688,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="s">
         <v>79</v>
       </c>
@@ -2554,7 +1810,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="s">
         <v>83</v>
       </c>
@@ -2676,7 +1932,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="s">
         <v>93</v>
       </c>
@@ -2798,7 +2054,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="s">
         <v>99</v>
       </c>
@@ -2920,7 +2176,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.15">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="s">
         <v>101</v>
       </c>
@@ -3043,48 +2299,53 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555551" footer="0.51180555555555551"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter alignWithMargins="0"/>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E25" activeCellId="1" sqref="E12:E22 E23:E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="16.875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="20.375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="21.75" style="8" customWidth="1"/>
-    <col min="4" max="4" width="16.25" style="8" customWidth="1"/>
-    <col min="5" max="5" width="16.875" style="8" customWidth="1"/>
-    <col min="6" max="6" width="31.625" style="8" customWidth="1"/>
-    <col min="7" max="7" width="19.625" style="8" customWidth="1"/>
-    <col min="8" max="8" width="18.75" style="8" customWidth="1"/>
-    <col min="9" max="9" width="15.75" style="8" customWidth="1"/>
-    <col min="10" max="10" width="17.75" style="8" customWidth="1"/>
-    <col min="11" max="11" width="21.75" style="8" customWidth="1"/>
-    <col min="12" max="12" width="20.625" style="8" customWidth="1"/>
-    <col min="13" max="13" width="26.75" style="8" customWidth="1"/>
-    <col min="14" max="16384" width="10.625" style="8"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="8" width="16.872641509434"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="8" width="20.377358490566"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="8" width="21.75"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="8" width="16.25"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="8" width="16.872641509434"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="8" width="31.627358490566"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="8" width="19.627358490566"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="8" width="18.7547169811321"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="8" width="15.75"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="8" width="17.7452830188679"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="8" width="21.75"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="8" width="20.627358490566"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="8" width="26.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="14" style="8" width="10.622641509434"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="28.5" x14ac:dyDescent="0.15">
-      <c r="A1" s="22" t="s">
-        <v>118</v>
-      </c>
-      <c r="B1" s="23" t="s">
+    <row r="1" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="20" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="22" t="s">
         <v>43</v>
       </c>
       <c r="D1" s="20" t="s">
@@ -3115,18 +2376,18 @@
         <v>99</v>
       </c>
       <c r="M1" s="20" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.15">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="25" t="s">
-        <v>120</v>
+        <v>111</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>112</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>45</v>
@@ -3146,8 +2407,8 @@
       <c r="I2" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J2" s="25" t="s">
-        <v>139</v>
+      <c r="J2" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>49</v>
@@ -3159,15 +2420,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>124</v>
+      <c r="B3" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>111</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>45</v>
@@ -3187,8 +2448,8 @@
       <c r="I3" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J3" s="25" t="s">
-        <v>139</v>
+      <c r="J3" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>49</v>
@@ -3200,15 +2461,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="C4" s="25" t="s">
-        <v>122</v>
+      <c r="B4" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>112</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>45</v>
@@ -3228,8 +2489,8 @@
       <c r="I4" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J4" s="25" t="s">
-        <v>139</v>
+      <c r="J4" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>49</v>
@@ -3241,15 +2502,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="C5" s="25" t="s">
-        <v>123</v>
+      <c r="B5" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>111</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>45</v>
@@ -3269,8 +2530,8 @@
       <c r="I5" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J5" s="25" t="s">
-        <v>139</v>
+      <c r="J5" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>49</v>
@@ -3282,15 +2543,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="C6" s="25" t="s">
-        <v>124</v>
+      <c r="B6" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="23" t="s">
+        <v>111</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>45</v>
@@ -3310,8 +2571,8 @@
       <c r="I6" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J6" s="25" t="s">
-        <v>139</v>
+      <c r="J6" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>49</v>
@@ -3323,15 +2584,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="C7" s="25" t="s">
-        <v>123</v>
+      <c r="B7" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="23" t="s">
+        <v>111</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>45</v>
@@ -3351,8 +2612,8 @@
       <c r="I7" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J7" s="25" t="s">
-        <v>139</v>
+      <c r="J7" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>49</v>
@@ -3364,15 +2625,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" s="25" t="s">
-        <v>125</v>
+      <c r="B8" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8" s="23" t="s">
+        <v>111</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>45</v>
@@ -3392,8 +2653,8 @@
       <c r="I8" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J8" s="25" t="s">
-        <v>139</v>
+      <c r="J8" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>49</v>
@@ -3405,15 +2666,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="C9" s="25" t="s">
-        <v>125</v>
+      <c r="B9" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>111</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>45</v>
@@ -3433,8 +2694,8 @@
       <c r="I9" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J9" s="25" t="s">
-        <v>139</v>
+      <c r="J9" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>49</v>
@@ -3446,15 +2707,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="C10" s="25" t="s">
-        <v>125</v>
+      <c r="B10" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="23" t="s">
+        <v>111</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>45</v>
@@ -3474,8 +2735,8 @@
       <c r="I10" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J10" s="25" t="s">
-        <v>139</v>
+      <c r="J10" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="K10" s="10" t="s">
         <v>49</v>
@@ -3487,15 +2748,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="26" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" s="25" t="s">
-        <v>122</v>
+      <c r="B11" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>41</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>45</v>
@@ -3515,8 +2776,8 @@
       <c r="I11" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="J11" s="25" t="s">
-        <v>139</v>
+      <c r="J11" s="23" t="s">
+        <v>91</v>
       </c>
       <c r="K11" s="10" t="s">
         <v>49</v>
@@ -3528,15 +2789,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="C12" s="26" t="s">
-        <v>127</v>
+      <c r="B12" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>112</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>45</v>
@@ -3556,8 +2817,8 @@
       <c r="I12" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="J12" s="26" t="s">
-        <v>138</v>
+      <c r="J12" s="24" t="s">
+        <v>113</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>49</v>
@@ -3569,15 +2830,15 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="13" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="C13" s="26" t="s">
-        <v>126</v>
+      <c r="B13" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>112</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>45</v>
@@ -3597,8 +2858,8 @@
       <c r="I13" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="J13" s="26" t="s">
-        <v>137</v>
+      <c r="J13" s="24" t="s">
+        <v>114</v>
       </c>
       <c r="K13" s="10" t="s">
         <v>49</v>
@@ -3610,15 +2871,15 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="14" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="C14" s="26" t="s">
-        <v>126</v>
+      <c r="B14" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>112</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>45</v>
@@ -3638,8 +2899,8 @@
       <c r="I14" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="J14" s="26" t="s">
-        <v>136</v>
+      <c r="J14" s="24" t="s">
+        <v>115</v>
       </c>
       <c r="K14" s="10" t="s">
         <v>49</v>
@@ -3651,15 +2912,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="15" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="C15" s="26" t="s">
-        <v>126</v>
+      <c r="B15" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>112</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>45</v>
@@ -3692,15 +2953,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="16" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="C16" s="26" t="s">
-        <v>126</v>
+      <c r="B16" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>112</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>45</v>
@@ -3733,15 +2994,15 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>126</v>
+      <c r="B17" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C17" s="24" t="s">
+        <v>112</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>46</v>
@@ -3770,24 +3031,24 @@
       <c r="L17" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="M17" s="21" t="s">
+      <c r="M17" s="25" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="C18" s="26" t="s">
-        <v>125</v>
+      <c r="B18" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C18" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="25" t="s">
         <v>52</v>
       </c>
       <c r="F18" s="10" t="s">
@@ -3811,19 +3072,19 @@
       <c r="L18" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="M18" s="21" t="s">
+      <c r="M18" s="25" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="C19" s="26" t="s">
-        <v>125</v>
+      <c r="B19" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>46</v>
@@ -3856,15 +3117,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="C20" s="26" t="s">
-        <v>125</v>
+      <c r="B20" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>46</v>
@@ -3897,15 +3158,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="C21" s="26" t="s">
-        <v>125</v>
+      <c r="B21" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>46</v>
@@ -3938,15 +3199,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>125</v>
+      <c r="B22" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>46</v>
@@ -3979,15 +3240,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="C23" s="26" t="s">
-        <v>125</v>
+      <c r="B23" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C23" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>46</v>
@@ -4020,15 +3281,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="C24" s="26" t="s">
-        <v>125</v>
+      <c r="B24" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>47</v>
@@ -4061,15 +3322,15 @@
         <v>107</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="26" t="s">
-        <v>129</v>
-      </c>
-      <c r="C25" s="26" t="s">
-        <v>130</v>
+      <c r="B25" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>112</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>48</v>
@@ -4102,15 +3363,15 @@
         <v>106</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C26" s="26" t="s">
-        <v>121</v>
+      <c r="B26" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>49</v>
@@ -4121,8 +3382,8 @@
       <c r="F26" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="G26" s="21" t="s">
-        <v>142</v>
+      <c r="G26" s="25" t="s">
+        <v>116</v>
       </c>
       <c r="H26" s="10" t="s">
         <v>51</v>
@@ -4143,15 +3404,15 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C27" s="26" t="s">
-        <v>121</v>
+      <c r="B27" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C27" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>49</v>
@@ -4162,8 +3423,8 @@
       <c r="F27" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="G27" s="28" t="s">
-        <v>143</v>
+      <c r="G27" s="26" t="s">
+        <v>117</v>
       </c>
       <c r="H27" s="10" t="s">
         <v>51</v>
@@ -4184,15 +3445,15 @@
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C28" s="26" t="s">
-        <v>121</v>
+      <c r="B28" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C28" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>45</v>
@@ -4225,15 +3486,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="27" t="s">
-        <v>141</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C29" s="26" t="s">
-        <v>121</v>
+        <v>118</v>
+      </c>
+      <c r="B29" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>45</v>
@@ -4266,15 +3527,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C30" s="26" t="s">
-        <v>121</v>
+      <c r="B30" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>45</v>
@@ -4307,15 +3568,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C31" s="26" t="s">
-        <v>121</v>
+      <c r="B31" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>45</v>
@@ -4348,15 +3609,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C32" s="26" t="s">
-        <v>121</v>
+      <c r="B32" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>45</v>
@@ -4389,15 +3650,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C33" s="26" t="s">
-        <v>121</v>
+      <c r="B33" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>45</v>
@@ -4430,15 +3691,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C34" s="26" t="s">
-        <v>121</v>
+      <c r="B34" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>45</v>
@@ -4471,15 +3732,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C35" s="26" t="s">
-        <v>121</v>
+      <c r="B35" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>45</v>
@@ -4502,8 +3763,8 @@
       <c r="J35" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="K35" s="26" t="s">
-        <v>135</v>
+      <c r="K35" s="24" t="s">
+        <v>96</v>
       </c>
       <c r="L35" s="10" t="s">
         <v>100</v>
@@ -4512,15 +3773,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C36" s="26" t="s">
-        <v>121</v>
+      <c r="B36" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>45</v>
@@ -4553,15 +3814,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="C37" s="26" t="s">
-        <v>121</v>
+      <c r="B37" s="24" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="24" t="s">
+        <v>111</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>45</v>
@@ -4594,58 +3855,54 @@
         <v>102</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B38" s="26" t="s">
-        <v>132</v>
-      </c>
-      <c r="C38" s="26" t="s">
-        <v>133</v>
+        <v>119</v>
+      </c>
+      <c r="B38" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="C38" s="24" t="s">
+        <v>112</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>112</v>
+        <v>73</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>113</v>
-      </c>
-      <c r="J38" s="26" t="s">
-        <v>140</v>
+        <v>122</v>
+      </c>
+      <c r="J38" s="24" t="s">
+        <v>123</v>
       </c>
       <c r="K38" s="10" t="s">
-        <v>114</v>
+        <v>49</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="M38" s="10" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <headerFooter alignWithMargins="0">
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
   </headerFooter>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>